<commit_message>
0002: Changes to the user interface, connection to the database and creation of the first beneficiary model
</commit_message>
<xml_diff>
--- a/db_register/Registro_beneficiarios.xlsx
+++ b/db_register/Registro_beneficiarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>NOMBRES Y APELLIDOS COMPLETOS</t>
   </si>
@@ -134,6 +134,24 @@
   </si>
   <si>
     <t>call 23 23 23</t>
+  </si>
+  <si>
+    <t>Jhan Carlos Ortiz</t>
+  </si>
+  <si>
+    <t>64646464</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Villa del lago</t>
+  </si>
+  <si>
+    <t>call 12 12 12</t>
+  </si>
+  <si>
+    <t>646464</t>
   </si>
 </sst>
 </file>
@@ -1348,19 +1366,31 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>3</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+    <row r="15">
+      <c r="B15" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H15" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s" s="0">
+        <v>43</v>
+      </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">

</xml_diff>